<commit_message>
la til siste eksamen
</commit_message>
<xml_diff>
--- a/diverse/tidsplan-H24.xlsx
+++ b/diverse/tidsplan-H24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\met4\diverse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2265DE-0702-4361-9037-03142B13DFE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6376FF-BF5C-49C3-A402-B2DAF1E8246A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -147,10 +147,10 @@
     <t>14.11: Speedrun dataanalyser</t>
   </si>
   <si>
-    <t>Mandag 10:15 - 11:00</t>
-  </si>
-  <si>
     <t>Torsdag 12:15 - 14:00</t>
+  </si>
+  <si>
+    <t>Mandag 10:15 - 12:00</t>
   </si>
 </sst>
 </file>
@@ -484,7 +484,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -502,10 +502,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
         <v>40</v>
-      </c>
-      <c r="D1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>